<commit_message>
Updated documentation and added ReadMe files for Biological Data and Climate Data folders
</commit_message>
<xml_diff>
--- a/Extensions beyond manuscript/Insect database.xlsx
+++ b/Extensions beyond manuscript/Insect database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c.johnson/Documents/GitHub/Johnson_Insect_Responses/Extensions beyond manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEAE3BC-FC95-1E44-9269-2B732D0F1BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FF62FD-C996-AF4E-B9C3-CDF5A9C684DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="1460" windowWidth="34300" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17720" yWindow="860" windowWidth="16840" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data base" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="345">
   <si>
     <t>Species</t>
   </si>
@@ -1210,6 +1210,18 @@
   </si>
   <si>
     <t>Not used because of poor fits for juvenile mortality data</t>
+  </si>
+  <si>
+    <t>Adelphocoris fasciaticollis</t>
+  </si>
+  <si>
+    <t>Adelphocoris lineolatus</t>
+  </si>
+  <si>
+    <t>China Tianjin</t>
+  </si>
+  <si>
+    <t>Did not want to use same temperature response data for two locations</t>
   </si>
 </sst>
 </file>
@@ -2108,10 +2120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="J7" sqref="A7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2316,22 +2328,22 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>197</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
       </c>
       <c r="D6">
-        <v>33.33</v>
-      </c>
-      <c r="E6">
-        <v>120.75</v>
+        <v>39.53</v>
+      </c>
+      <c r="E6" s="5">
+        <v>116.7</v>
       </c>
       <c r="F6" t="s">
         <v>40</v>
       </c>
-      <c r="G6" t="s">
-        <v>37</v>
+      <c r="G6" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="H6" t="s">
         <v>6</v>
@@ -2346,12 +2358,12 @@
         <v>6</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -2366,7 +2378,7 @@
         <v>120.75</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
         <v>37</v>
@@ -2389,22 +2401,22 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8">
-        <v>39.880000000000003</v>
+        <v>35.53</v>
       </c>
       <c r="E8">
-        <v>117.17</v>
+        <v>114.42</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
         <v>37</v>
@@ -2420,9 +2432,6 @@
       </c>
       <c r="K8">
         <v>6</v>
-      </c>
-      <c r="L8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -2430,22 +2439,22 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
       </c>
       <c r="D9">
-        <v>35.53</v>
+        <v>33.33</v>
       </c>
       <c r="E9">
-        <v>114.42</v>
+        <v>120.75</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
       </c>
-      <c r="G9" t="s">
-        <v>37</v>
+      <c r="G9" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="H9" t="s">
         <v>6</v>
@@ -2460,33 +2469,33 @@
         <v>6</v>
       </c>
       <c r="L9" t="s">
-        <v>42</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>341</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>33</v>
+        <v>343</v>
+      </c>
+      <c r="C10" t="s">
+        <v>274</v>
       </c>
       <c r="D10">
-        <v>38.380000000000003</v>
+        <v>38.549999999999997</v>
       </c>
       <c r="E10">
-        <v>23.14</v>
+        <v>117.38</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
       </c>
       <c r="H10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I10" t="s">
         <v>5</v>
@@ -2495,36 +2504,33 @@
         <v>141</v>
       </c>
       <c r="K10">
-        <v>5</v>
-      </c>
-      <c r="L10" t="s">
-        <v>241</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>342</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
+        <v>197</v>
+      </c>
+      <c r="C11" t="s">
+        <v>274</v>
       </c>
       <c r="D11">
-        <v>38.380000000000003</v>
+        <v>39.880000000000003</v>
       </c>
       <c r="E11">
-        <v>23.14</v>
+        <v>117.17</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
       </c>
       <c r="H11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I11" t="s">
         <v>5</v>
@@ -2533,7 +2539,7 @@
         <v>141</v>
       </c>
       <c r="K11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L11" t="s">
         <v>241</v>
@@ -2541,69 +2547,72 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>244</v>
+        <v>16</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="D12">
-        <v>-21.23</v>
+        <v>38.380000000000003</v>
       </c>
       <c r="E12">
-        <v>-44.98</v>
+        <v>23.14</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" t="s">
-        <v>37</v>
+        <v>48</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="H12" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="K12">
         <v>5</v>
+      </c>
+      <c r="L12" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>244</v>
+        <v>16</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="D13">
-        <v>-21.23</v>
+        <v>38.380000000000003</v>
       </c>
       <c r="E13">
-        <v>-44.98</v>
+        <v>23.14</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" t="s">
-        <v>37</v>
+        <v>48</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="H13" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="K13">
         <v>5</v>
@@ -2611,7 +2620,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -2646,98 +2655,95 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>99</v>
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>244</v>
       </c>
       <c r="D15">
-        <v>33.619999999999997</v>
+        <v>-21.23</v>
       </c>
       <c r="E15">
-        <v>133.66999999999999</v>
+        <v>-44.98</v>
       </c>
       <c r="F15" t="s">
-        <v>327</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>38</v>
+        <v>47</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
       </c>
       <c r="H15" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="I15" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>141</v>
+        <v>83</v>
       </c>
       <c r="K15">
-        <v>6</v>
-      </c>
-      <c r="L15" t="s">
-        <v>241</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D16">
-        <v>33.42</v>
+        <v>-21.23</v>
       </c>
       <c r="E16">
-        <v>-90.9</v>
+        <v>-44.98</v>
       </c>
       <c r="F16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>38</v>
+        <v>47</v>
+      </c>
+      <c r="G16" t="s">
+        <v>37</v>
       </c>
       <c r="H16" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="I16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>141</v>
+        <v>83</v>
       </c>
       <c r="K16">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L16" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>212</v>
+        <v>99</v>
       </c>
       <c r="D17">
-        <v>35.380000000000003</v>
+        <v>33.619999999999997</v>
       </c>
       <c r="E17">
-        <v>140.07</v>
+        <v>133.66999999999999</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>327</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>38</v>
@@ -2746,36 +2752,36 @@
         <v>46</v>
       </c>
       <c r="I17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="K17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L17" t="s">
-        <v>340</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>198</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>213</v>
+        <v>208</v>
+      </c>
+      <c r="C18" t="s">
+        <v>243</v>
       </c>
       <c r="D18">
-        <v>35.380000000000003</v>
+        <v>33.42</v>
       </c>
       <c r="E18">
-        <v>140.07</v>
+        <v>-90.9</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>38</v>
@@ -2784,10 +2790,10 @@
         <v>46</v>
       </c>
       <c r="I18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="K18">
         <v>7</v>
@@ -2798,7 +2804,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
         <v>198</v>
@@ -2828,7 +2834,7 @@
         <v>83</v>
       </c>
       <c r="K19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L19" t="s">
         <v>340</v>
@@ -2836,13 +2842,13 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
         <v>198</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D20">
         <v>35.380000000000003</v>
@@ -2866,7 +2872,7 @@
         <v>83</v>
       </c>
       <c r="K20">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L20" t="s">
         <v>340</v>
@@ -2874,60 +2880,60 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>200</v>
-      </c>
-      <c r="C21" t="s">
-        <v>334</v>
+        <v>198</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>212</v>
       </c>
       <c r="D21">
-        <v>54.02</v>
+        <v>35.380000000000003</v>
       </c>
       <c r="E21">
-        <v>-0.97</v>
+        <v>140.07</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" t="s">
-        <v>37</v>
+        <v>50</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="H21" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K21">
         <v>6</v>
       </c>
-      <c r="I21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K21">
-        <v>5</v>
-      </c>
       <c r="L21" t="s">
-        <v>242</v>
+        <v>340</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>205</v>
-      </c>
-      <c r="C22" t="s">
-        <v>214</v>
+        <v>198</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>212</v>
       </c>
       <c r="D22">
-        <v>25.47</v>
+        <v>35.380000000000003</v>
       </c>
       <c r="E22">
-        <v>-80.48</v>
+        <v>140.07</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>38</v>
@@ -2939,39 +2945,39 @@
         <v>8</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="K22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L22" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C23" t="s">
-        <v>233</v>
+        <v>334</v>
       </c>
       <c r="D23">
-        <v>26.14</v>
+        <v>54.02</v>
       </c>
       <c r="E23">
-        <v>-81.790000000000006</v>
+        <v>-0.97</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G23" t="s">
         <v>37</v>
       </c>
       <c r="H23" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="I23" t="s">
         <v>8</v>
@@ -2980,30 +2986,33 @@
         <v>83</v>
       </c>
       <c r="K23">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="L23" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>214</v>
       </c>
       <c r="D24">
-        <v>26.14</v>
+        <v>25.47</v>
       </c>
       <c r="E24">
-        <v>-80.45</v>
+        <v>-80.48</v>
       </c>
       <c r="F24" t="s">
-        <v>62</v>
-      </c>
-      <c r="G24" t="s">
-        <v>37</v>
+        <v>60</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="H24" t="s">
         <v>46</v>
@@ -3012,33 +3021,33 @@
         <v>8</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="K24">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C25" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="D25">
-        <v>26.24</v>
+        <v>26.14</v>
       </c>
       <c r="E25">
-        <v>-80.12</v>
+        <v>-81.790000000000006</v>
       </c>
       <c r="F25" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>38</v>
+        <v>61</v>
+      </c>
+      <c r="G25" t="s">
+        <v>37</v>
       </c>
       <c r="H25" t="s">
         <v>46</v>
@@ -3047,33 +3056,30 @@
         <v>8</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="K25">
-        <v>7</v>
-      </c>
-      <c r="L25" t="s">
-        <v>256</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C26" t="s">
-        <v>234</v>
-      </c>
-      <c r="D26" s="5">
-        <v>-30.9</v>
+        <v>23</v>
+      </c>
+      <c r="D26">
+        <v>26.14</v>
       </c>
       <c r="E26">
-        <v>115.78</v>
+        <v>-80.45</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G26" t="s">
         <v>37</v>
@@ -3090,25 +3096,28 @@
       <c r="K26">
         <v>7</v>
       </c>
+      <c r="L26" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>221</v>
       </c>
       <c r="D27">
-        <v>33.69</v>
+        <v>26.24</v>
       </c>
       <c r="E27">
-        <v>-101.8</v>
+        <v>-80.12</v>
       </c>
       <c r="F27" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>38</v>
@@ -3120,39 +3129,36 @@
         <v>8</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="K27">
-        <v>6</v>
-      </c>
-      <c r="L27" t="s">
-        <v>340</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C28" t="s">
-        <v>235</v>
-      </c>
-      <c r="D28">
-        <v>52.62</v>
+        <v>234</v>
+      </c>
+      <c r="D28" s="5">
+        <v>-30.9</v>
       </c>
       <c r="E28">
-        <v>1.24</v>
+        <v>115.78</v>
       </c>
       <c r="F28" t="s">
-        <v>70</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>38</v>
+        <v>64</v>
+      </c>
+      <c r="G28" t="s">
+        <v>37</v>
       </c>
       <c r="H28" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="I28" t="s">
         <v>8</v>
@@ -3161,45 +3167,45 @@
         <v>83</v>
       </c>
       <c r="K28">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L28" t="s">
-        <v>249</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C29" t="s">
-        <v>235</v>
+        <v>25</v>
       </c>
       <c r="D29">
-        <v>52.62</v>
+        <v>33.69</v>
       </c>
       <c r="E29">
-        <v>1.24</v>
+        <v>-101.8</v>
       </c>
       <c r="F29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>38</v>
       </c>
       <c r="H29" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K29">
         <v>6</v>
-      </c>
-      <c r="I29" t="s">
-        <v>8</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K29">
-        <v>5</v>
       </c>
       <c r="L29" t="s">
         <v>249</v>
@@ -3207,25 +3213,25 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>202</v>
       </c>
       <c r="C30" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="D30">
-        <v>42.81</v>
+        <v>52.62</v>
       </c>
       <c r="E30">
-        <v>-82.23</v>
+        <v>1.24</v>
       </c>
       <c r="F30" t="s">
-        <v>71</v>
-      </c>
-      <c r="G30" t="s">
-        <v>37</v>
+        <v>70</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="H30" t="s">
         <v>6</v>
@@ -3237,30 +3243,33 @@
         <v>83</v>
       </c>
       <c r="K30">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="L30" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>202</v>
       </c>
       <c r="C31" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="D31">
-        <v>42.81</v>
+        <v>52.62</v>
       </c>
       <c r="E31">
-        <v>-82.23</v>
+        <v>1.24</v>
       </c>
       <c r="F31" t="s">
-        <v>71</v>
-      </c>
-      <c r="G31" t="s">
-        <v>37</v>
+        <v>70</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="H31" t="s">
         <v>6</v>
@@ -3272,33 +3281,33 @@
         <v>83</v>
       </c>
       <c r="K31">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>203</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="D32">
-        <v>-35.270000000000003</v>
+        <v>42.81</v>
       </c>
       <c r="E32">
-        <v>149.11000000000001</v>
+        <v>-82.23</v>
       </c>
       <c r="F32" t="s">
-        <v>72</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>38</v>
+        <v>71</v>
+      </c>
+      <c r="G32" t="s">
+        <v>37</v>
       </c>
       <c r="H32" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="I32" t="s">
         <v>8</v>
@@ -3309,34 +3318,31 @@
       <c r="K32">
         <v>6</v>
       </c>
-      <c r="L32" t="s">
-        <v>340</v>
-      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="D33">
-        <v>35.75</v>
+        <v>42.81</v>
       </c>
       <c r="E33">
-        <v>51.17</v>
+        <v>-82.23</v>
       </c>
       <c r="F33" t="s">
-        <v>73</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>38</v>
+        <v>71</v>
+      </c>
+      <c r="G33" t="s">
+        <v>37</v>
       </c>
       <c r="H33" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="I33" t="s">
         <v>8</v>
@@ -3353,28 +3359,28 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>246</v>
       </c>
       <c r="D34">
-        <v>36.07</v>
+        <v>-35.270000000000003</v>
       </c>
       <c r="E34">
-        <v>114.22</v>
+        <v>149.11000000000001</v>
       </c>
       <c r="F34" t="s">
-        <v>74</v>
-      </c>
-      <c r="G34" t="s">
-        <v>37</v>
+        <v>72</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="H34" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="I34" t="s">
         <v>8</v>
@@ -3385,31 +3391,34 @@
       <c r="K34">
         <v>6</v>
       </c>
+      <c r="L34" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>225</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>210</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D35">
-        <v>42.42</v>
+        <v>35.75</v>
       </c>
       <c r="E35">
-        <v>-76.53</v>
+        <v>51.17</v>
       </c>
       <c r="F35" t="s">
-        <v>75</v>
-      </c>
-      <c r="G35" t="s">
-        <v>37</v>
+        <v>73</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="H35" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="I35" t="s">
         <v>8</v>
@@ -3423,22 +3432,22 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C36" t="s">
-        <v>247</v>
+        <v>25</v>
       </c>
       <c r="D36">
-        <v>38.93</v>
+        <v>36.07</v>
       </c>
       <c r="E36">
-        <v>-92.34</v>
+        <v>114.22</v>
       </c>
       <c r="F36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G36" t="s">
         <v>37</v>
@@ -3453,27 +3462,27 @@
         <v>83</v>
       </c>
       <c r="K36">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>225</v>
       </c>
       <c r="B37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C37" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="D37">
-        <v>38.93</v>
+        <v>42.42</v>
       </c>
       <c r="E37">
-        <v>-92.34</v>
+        <v>-76.53</v>
       </c>
       <c r="F37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G37" t="s">
         <v>37</v>
@@ -3488,18 +3497,18 @@
         <v>83</v>
       </c>
       <c r="K37">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
         <v>211</v>
       </c>
       <c r="C38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D38">
         <v>38.93</v>
@@ -3527,31 +3536,31 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>53</v>
+      <c r="A39" t="s">
+        <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>332</v>
+        <v>211</v>
       </c>
       <c r="C39" t="s">
-        <v>334</v>
-      </c>
-      <c r="D39" s="5">
-        <v>45.38</v>
-      </c>
-      <c r="E39" s="5">
-        <v>-75.69</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>38</v>
+        <v>247</v>
+      </c>
+      <c r="D39">
+        <v>38.93</v>
+      </c>
+      <c r="E39">
+        <v>-92.34</v>
+      </c>
+      <c r="F39" t="s">
+        <v>76</v>
+      </c>
+      <c r="G39" t="s">
+        <v>37</v>
       </c>
       <c r="H39" t="s">
         <v>6</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="I39" t="s">
         <v>8</v>
       </c>
       <c r="J39" s="2" t="s">
@@ -3560,86 +3569,156 @@
       <c r="K39">
         <v>7</v>
       </c>
-      <c r="L39" t="s">
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
+        <v>211</v>
+      </c>
+      <c r="C40" t="s">
+        <v>248</v>
+      </c>
+      <c r="D40">
+        <v>38.93</v>
+      </c>
+      <c r="E40">
+        <v>-92.34</v>
+      </c>
+      <c r="F40" t="s">
+        <v>76</v>
+      </c>
+      <c r="G40" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" t="s">
+        <v>6</v>
+      </c>
+      <c r="I40" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K40">
+        <v>7</v>
+      </c>
+      <c r="L40" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
+        <v>332</v>
+      </c>
+      <c r="C41" t="s">
+        <v>334</v>
+      </c>
+      <c r="D41" s="5">
+        <v>45.38</v>
+      </c>
+      <c r="E41" s="5">
+        <v>-75.69</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H41" t="s">
+        <v>6</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K41">
+        <v>7</v>
+      </c>
+      <c r="L41" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" t="s">
         <v>273</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>274</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D42" s="5">
         <f>50+43/60</f>
         <v>50.716666666666669</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E42" s="7">
         <f>-120-25/60</f>
         <v>-120.41666666666667</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="G42" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H42" t="s">
         <v>6</v>
       </c>
-      <c r="I40" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K40">
-        <v>5</v>
-      </c>
-      <c r="L40" t="s">
+      <c r="I42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K42">
+        <v>5</v>
+      </c>
+      <c r="L42" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D41">
+      <c r="D43">
         <v>45.41</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E43" s="2">
         <v>-73.94</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="G43" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H43" t="s">
         <v>6</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K41">
+      <c r="I43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K43">
         <v>7</v>
-      </c>
-      <c r="L41" t="s">
-        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -3652,7 +3731,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:D30"/>
+      <selection activeCell="A8" sqref="A8:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3810,7 +3889,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -3833,7 +3912,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -3856,7 +3935,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="2" t="s">
         <v>290</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -4293,10 +4372,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84:G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5668,7 +5747,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>224</v>
       </c>
@@ -5685,7 +5764,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>326</v>
       </c>
@@ -5702,7 +5781,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>336</v>
       </c>
@@ -5719,7 +5798,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>335</v>
       </c>
@@ -5735,12 +5814,7 @@
       <c r="E84" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="F84" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G84">
-        <v>-22.11</v>
-      </c>
+      <c r="F84" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>